<commit_message>
Collected as much data for 2018 including fantasy points -- skips some players
Skipping some players due to version error with URL. All player files can be found in 2018_data directory with data and fantasy points from 2018 season.
</commit_message>
<xml_diff>
--- a/2018_data/Allen_Lazard2018.xlsx
+++ b/2018_data/Allen_Lazard2018.xlsx
@@ -12,47 +12,6 @@
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
-  <si>
-    <t>https://www.pro-football-reference.com/players/L/LazaAl00/gamelog/2018/</t>
-  </si>
-  <si>
-    <t>2018-12-30</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>23.019</t>
-  </si>
-  <si>
-    <t>GNB</t>
-  </si>
-  <si>
-    <t>DET</t>
-  </si>
-  <si>
-    <t>L 0-31</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>7.00</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>100.0%</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -386,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -394,50 +353,91 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:16">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s"/>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s"/>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" t="s">
-        <v>11</v>
-      </c>
-      <c r="P1" t="s">
-        <v>9</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Lazard</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Allen</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>WR</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>2018-12-30</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>23.019</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>GNB</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr"/>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>DET</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>L 0-31</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr"/>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>7.00</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>100.0%</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>7.00</t>
+        </is>
+      </c>
+      <c r="S1" t="n">
+        <v>0.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>